<commit_message>
Passes first test (runs to completion without altering behavior).
</commit_message>
<xml_diff>
--- a/testings/CoreV7.0-BiomassSuccession6.0/SppEcoregionData.xlsx
+++ b/testings/CoreV7.0-BiomassSuccession6.0/SppEcoregionData.xlsx
@@ -74,9 +74,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>EcoregionIndex</t>
-  </si>
-  <si>
     <t>SpeciesCode</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>BiomassMax</t>
+  </si>
+  <si>
+    <t>EcoregionName</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -418,22 +420,22 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final tweaks before release.
</commit_message>
<xml_diff>
--- a/testings/CoreV7.0-BiomassSuccession6.0/SppEcoregionData.xlsx
+++ b/testings/CoreV7.0-BiomassSuccession6.0/SppEcoregionData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>abiebals</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>0.9</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F2">
         <v>886</v>
@@ -475,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F3">
         <v>1175</v>
@@ -498,7 +498,7 @@
         <v>0.82</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F4">
         <v>1106</v>
@@ -521,7 +521,7 @@
         <v>0.64</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F5">
         <v>1202</v>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F6">
         <v>1202</v>
@@ -567,7 +567,7 @@
         <v>0.18</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F7">
         <v>1202</v>
@@ -590,7 +590,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F8">
         <v>969</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F9">
         <v>1130</v>
@@ -636,7 +636,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F10">
         <v>1017</v>
@@ -659,7 +659,7 @@
         <v>0.72</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F11">
         <v>1090</v>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F12">
         <v>1078</v>
@@ -705,7 +705,7 @@
         <v>0.96</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F13">
         <v>1096</v>
@@ -728,7 +728,7 @@
         <v>0.66</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F14">
         <v>1017</v>
@@ -751,7 +751,7 @@
         <v>0.76</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F15">
         <v>1090</v>
@@ -774,12 +774,357 @@
         <v>0.54</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F16">
         <v>1078</v>
       </c>
       <c r="G16">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.9</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>886</v>
+      </c>
+      <c r="G17">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1175</v>
+      </c>
+      <c r="G18">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0.82</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1106</v>
+      </c>
+      <c r="G19">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0.64</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1202</v>
+      </c>
+      <c r="G20">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1202</v>
+      </c>
+      <c r="G21">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>0.18</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1202</v>
+      </c>
+      <c r="G22">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>969</v>
+      </c>
+      <c r="G23">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1130</v>
+      </c>
+      <c r="G24">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1017</v>
+      </c>
+      <c r="G25">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>0.72</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1090</v>
+      </c>
+      <c r="G26">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1078</v>
+      </c>
+      <c r="G27">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>0.96</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1096</v>
+      </c>
+      <c r="G28">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>0.66</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1017</v>
+      </c>
+      <c r="G29">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>0.76</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1090</v>
+      </c>
+      <c r="G30">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>0.54</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1078</v>
+      </c>
+      <c r="G31">
         <v>26000</v>
       </c>
     </row>

</xml_diff>